<commit_message>
added some sign images to the excel sheet
</commit_message>
<xml_diff>
--- a/final_WWashington_data_images/Washington_sign_images.xlsx
+++ b/final_WWashington_data_images/Washington_sign_images.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omkar\Desktop\Data_Science_new_folder\DataScienceProject\final_WWashington_data_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BA98F3-0AF8-4237-BA6B-9ECE921E04F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EC0A19-8856-4035-821A-9FF711D866DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Number</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>row2_b.PNG</t>
+  </si>
+  <si>
+    <t>row2_c.PNG</t>
+  </si>
+  <si>
+    <t>row2_d.PNG</t>
+  </si>
+  <si>
+    <t>row2_e.PNG</t>
   </si>
 </sst>
 </file>
@@ -360,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,6 +418,42 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
made changes in the file  Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/final_WWashington_data_images/Washington_sign_images.xlsx
+++ b/final_WWashington_data_images/Washington_sign_images.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omkar\Desktop\Data_Science_new_folder\DataScienceProject\final_WWashington_data_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EC0A19-8856-4035-821A-9FF711D866DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA6D694-6046-4DDA-82EE-0F12D3323F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,23 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Number</t>
   </si>
   <si>
-    <t>Image_id</t>
-  </si>
-  <si>
     <t>class_type</t>
   </si>
   <si>
     <t>data_frame_row_number</t>
   </si>
   <si>
-    <t>row2_a.PNG</t>
-  </si>
-  <si>
     <t>row2_b.PNG</t>
   </si>
   <si>
@@ -52,6 +46,24 @@
   </si>
   <si>
     <t>row2_e.PNG</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Accident Id</t>
+  </si>
+  <si>
+    <t>A-2827637</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image_link   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  </t>
+  </si>
+  <si>
+    <t>00001.PNG</t>
   </si>
 </sst>
 </file>
@@ -369,34 +381,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.21875" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="2" max="3" width="33.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -404,54 +419,67 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
-        <v>8</v>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleted the old image files and made changes in the xls sheet
</commit_message>
<xml_diff>
--- a/final_WWashington_data_images/Washington_sign_images.xlsx
+++ b/final_WWashington_data_images/Washington_sign_images.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omkar\Desktop\Data_Science_new_folder\DataScienceProject\final_WWashington_data_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA6D694-6046-4DDA-82EE-0F12D3323F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC62A32B-C953-4C44-98EF-EEA35227379B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Number</t>
   </si>
@@ -36,21 +36,6 @@
     <t>data_frame_row_number</t>
   </si>
   <si>
-    <t>row2_b.PNG</t>
-  </si>
-  <si>
-    <t>row2_c.PNG</t>
-  </si>
-  <si>
-    <t>row2_d.PNG</t>
-  </si>
-  <si>
-    <t>row2_e.PNG</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>Accident Id</t>
   </si>
   <si>
@@ -63,7 +48,28 @@
     <t xml:space="preserve">                  </t>
   </si>
   <si>
-    <t>00001.PNG</t>
+    <t>00001.png</t>
+  </si>
+  <si>
+    <t>0002.png</t>
+  </si>
+  <si>
+    <t>0003.png</t>
+  </si>
+  <si>
+    <t>0004.png</t>
+  </si>
+  <si>
+    <t>0005.png</t>
+  </si>
+  <si>
+    <t>0006.png</t>
+  </si>
+  <si>
+    <t>no class</t>
+  </si>
+  <si>
+    <t>0007.png</t>
   </si>
 </sst>
 </file>
@@ -381,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -402,10 +408,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -419,10 +425,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -432,8 +438,11 @@
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -443,8 +452,11 @@
       <c r="B4">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -454,8 +466,11 @@
       <c r="B5">
         <v>2</v>
       </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>14</v>
@@ -468,18 +483,50 @@
       <c r="B6">
         <v>2</v>
       </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
       <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made change to xl sheet
</commit_message>
<xml_diff>
--- a/final_WWashington_data_images/Washington_sign_images.xlsx
+++ b/final_WWashington_data_images/Washington_sign_images.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omkar\Desktop\Data_Science_new_folder\DataScienceProject\final_WWashington_data_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC62A32B-C953-4C44-98EF-EEA35227379B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9923D3B7-FCFC-4D9B-8789-7A3752E9E515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -390,7 +390,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added more streetview images
</commit_message>
<xml_diff>
--- a/final_WWashington_data_images/Washington_sign_images.xlsx
+++ b/final_WWashington_data_images/Washington_sign_images.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omkar\Desktop\Data_Science_new_folder\DataScienceProject\final_WWashington_data_images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshamakumar/Downloads/5305-DS/Homework/DataScienceProject/final_WWashington_data_images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194C5672-546C-4FF9-A0BF-EBE36C488CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F90504A-CF72-3E4F-A31A-B61E08E89435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
   <si>
     <t>Number</t>
   </si>
@@ -118,16 +118,107 @@
   </si>
   <si>
     <t>stop here sing- no class</t>
+  </si>
+  <si>
+    <t>A-2829033</t>
+  </si>
+  <si>
+    <t>1111.png</t>
+  </si>
+  <si>
+    <t>converging roads</t>
+  </si>
+  <si>
+    <t>1112.png</t>
+  </si>
+  <si>
+    <t>speed limit 60</t>
+  </si>
+  <si>
+    <t>1113.png</t>
+  </si>
+  <si>
+    <t>U-turn + Speed limit 20</t>
+  </si>
+  <si>
+    <t>A-2829014</t>
+  </si>
+  <si>
+    <t>1114.png</t>
+  </si>
+  <si>
+    <t>Ramp+Speed limit 50</t>
+  </si>
+  <si>
+    <t>1115.png</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>A-2828996</t>
+  </si>
+  <si>
+    <t>1116.png</t>
+  </si>
+  <si>
+    <t>Ramp+Speed limit 40</t>
+  </si>
+  <si>
+    <t>1117.png</t>
+  </si>
+  <si>
+    <t>1118.png</t>
+  </si>
+  <si>
+    <t>speed limit 45</t>
+  </si>
+  <si>
+    <t>Exit + Speed limit 25</t>
+  </si>
+  <si>
+    <t>A-2828857</t>
+  </si>
+  <si>
+    <t>1119.png</t>
+  </si>
+  <si>
+    <t>1120.png</t>
+  </si>
+  <si>
+    <t>speed limit 50</t>
+  </si>
+  <si>
+    <t>1121.png</t>
+  </si>
+  <si>
+    <t>crossroad</t>
+  </si>
+  <si>
+    <t>t-intersection</t>
+  </si>
+  <si>
+    <t>1122.png</t>
+  </si>
+  <si>
+    <t>1123.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,8 +244,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,20 +527,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="33.21875" customWidth="1"/>
+    <col min="2" max="3" width="33.1640625" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="30.77734375" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -479,7 +571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -493,7 +585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -507,7 +599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -524,7 +616,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -538,7 +630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -555,7 +647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -572,7 +664,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -589,7 +681,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -606,7 +698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -623,7 +715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -640,7 +732,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -657,7 +749,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -674,7 +766,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -691,7 +783,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -708,7 +800,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -725,7 +817,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -740,6 +832,221 @@
       </c>
       <c r="E18" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some more data
</commit_message>
<xml_diff>
--- a/final_WWashington_data_images/Washington_sign_images.xlsx
+++ b/final_WWashington_data_images/Washington_sign_images.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omkar\Desktop\Data_Science_new_folder\DataScienceProject\final_WWashington_data_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944521D2-609D-43A3-A182-28D2F484112C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA23E5B-0C64-478F-9F9D-F9F501D217DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>Number</t>
   </si>
@@ -109,6 +109,72 @@
   </si>
   <si>
     <t>34 maybe</t>
+  </si>
+  <si>
+    <t>A-2827768</t>
+  </si>
+  <si>
+    <t>0016.png</t>
+  </si>
+  <si>
+    <t>0017.png</t>
+  </si>
+  <si>
+    <t>0018.png</t>
+  </si>
+  <si>
+    <t>0019.png</t>
+  </si>
+  <si>
+    <t>A-2827812</t>
+  </si>
+  <si>
+    <t>0020.png</t>
+  </si>
+  <si>
+    <t>0021.png</t>
+  </si>
+  <si>
+    <t>0022.png</t>
+  </si>
+  <si>
+    <t>A-2827885</t>
+  </si>
+  <si>
+    <t>0023.png</t>
+  </si>
+  <si>
+    <t>0024.png</t>
+  </si>
+  <si>
+    <t>0025.png</t>
+  </si>
+  <si>
+    <t>0026.png</t>
+  </si>
+  <si>
+    <t>0027.png</t>
+  </si>
+  <si>
+    <t>0028.png</t>
+  </si>
+  <si>
+    <t>0029.png</t>
+  </si>
+  <si>
+    <t>0030.png</t>
+  </si>
+  <si>
+    <t>0031.png</t>
+  </si>
+  <si>
+    <t>A-2828052</t>
+  </si>
+  <si>
+    <t>A-2828231</t>
+  </si>
+  <si>
+    <t>A-2828314</t>
   </si>
 </sst>
 </file>
@@ -434,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,105 +717,377 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B13">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>26</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B15">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
         <v>28</v>
       </c>
-      <c r="B16">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E16">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B17">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E17">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>30</v>
       </c>
-      <c r="B18">
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>26</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>21</v>
+      </c>
+      <c r="B31">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32">
         <v>23</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C32" t="s">
         <v>23</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
         <v>26</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E34" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added remaining pictures and renumbered correctly
</commit_message>
<xml_diff>
--- a/final_WWashington_data_images/Washington_sign_images.xlsx
+++ b/final_WWashington_data_images/Washington_sign_images.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omkar\Desktop\Data_Science_new_folder\DataScienceProject\final_WWashington_data_images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshamakumar/Downloads/5305-DS/Homework/DataScienceProject/final_WWashington_data_images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA23E5B-0C64-478F-9F9D-F9F501D217DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6657C34-967D-5B48-AE58-D613EDEB4D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="83">
   <si>
     <t>Number</t>
   </si>
@@ -84,30 +84,12 @@
     <t>A-2829033</t>
   </si>
   <si>
-    <t>1112.png</t>
-  </si>
-  <si>
-    <t>1113.png</t>
-  </si>
-  <si>
     <t>A-2829014</t>
   </si>
   <si>
-    <t>1114.png</t>
-  </si>
-  <si>
     <t>A-2828857</t>
   </si>
   <si>
-    <t>1121.png</t>
-  </si>
-  <si>
-    <t>1122.png</t>
-  </si>
-  <si>
-    <t>1123.png</t>
-  </si>
-  <si>
     <t>34 maybe</t>
   </si>
   <si>
@@ -175,13 +157,130 @@
   </si>
   <si>
     <t>A-2828314</t>
+  </si>
+  <si>
+    <t>0032.png</t>
+  </si>
+  <si>
+    <t>0033.png</t>
+  </si>
+  <si>
+    <t>0034.png</t>
+  </si>
+  <si>
+    <t>0035.png</t>
+  </si>
+  <si>
+    <t>0036.png</t>
+  </si>
+  <si>
+    <t>0037.png</t>
+  </si>
+  <si>
+    <t>A-2829809</t>
+  </si>
+  <si>
+    <t>0038.png</t>
+  </si>
+  <si>
+    <t>0039.png</t>
+  </si>
+  <si>
+    <t>0040.png</t>
+  </si>
+  <si>
+    <t>0041.png</t>
+  </si>
+  <si>
+    <t>0042.png</t>
+  </si>
+  <si>
+    <t>Spped limit 30</t>
+  </si>
+  <si>
+    <t>No pedestrian crossing</t>
+  </si>
+  <si>
+    <t>right turn</t>
+  </si>
+  <si>
+    <t>No parking</t>
+  </si>
+  <si>
+    <t>speed limit 30</t>
+  </si>
+  <si>
+    <t>A-2829794</t>
+  </si>
+  <si>
+    <t>0043.png</t>
+  </si>
+  <si>
+    <t>speed limit 40</t>
+  </si>
+  <si>
+    <t>A-2829776</t>
+  </si>
+  <si>
+    <t>00.44.png</t>
+  </si>
+  <si>
+    <t>right lane end</t>
+  </si>
+  <si>
+    <t>0045.png</t>
+  </si>
+  <si>
+    <t>exit + speed limit 25</t>
+  </si>
+  <si>
+    <t>0046.png</t>
+  </si>
+  <si>
+    <t>exit</t>
+  </si>
+  <si>
+    <t>0047.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop </t>
+  </si>
+  <si>
+    <t>0048.png</t>
+  </si>
+  <si>
+    <t>speed limit 25</t>
+  </si>
+  <si>
+    <t>0049.png</t>
+  </si>
+  <si>
+    <t>A-2829686</t>
+  </si>
+  <si>
+    <t>A-2829398</t>
+  </si>
+  <si>
+    <t>0050.png</t>
+  </si>
+  <si>
+    <t>0051.png</t>
+  </si>
+  <si>
+    <t>0052.png</t>
+  </si>
+  <si>
+    <t>roundabout</t>
+  </si>
+  <si>
+    <t>pedestrian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +291,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -500,20 +605,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="33.109375" customWidth="1"/>
+    <col min="2" max="3" width="33.1640625" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="30.77734375" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -530,7 +635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -547,7 +652,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -564,7 +669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -581,7 +686,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -598,7 +703,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -615,7 +720,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -632,7 +737,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -649,7 +754,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -666,7 +771,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>13</v>
       </c>
@@ -683,7 +788,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>14</v>
       </c>
@@ -700,7 +805,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>15</v>
       </c>
@@ -717,7 +822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>16</v>
       </c>
@@ -725,16 +830,16 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E13">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>17</v>
       </c>
@@ -742,16 +847,16 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E14">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>18</v>
       </c>
@@ -759,16 +864,16 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>19</v>
       </c>
@@ -776,16 +881,16 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E16">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20</v>
       </c>
@@ -793,16 +898,16 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E17">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>21</v>
       </c>
@@ -810,16 +915,16 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E18">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>22</v>
       </c>
@@ -827,16 +932,16 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E19">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>23</v>
       </c>
@@ -844,16 +949,16 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E20">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>24</v>
       </c>
@@ -861,16 +966,16 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E21">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>25</v>
       </c>
@@ -878,16 +983,16 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E22">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>26</v>
       </c>
@@ -895,16 +1000,16 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>27</v>
       </c>
@@ -912,16 +1017,16 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E24">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>28</v>
       </c>
@@ -929,16 +1034,16 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E25">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>29</v>
       </c>
@@ -946,16 +1051,16 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E26">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>30</v>
       </c>
@@ -963,16 +1068,16 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E27">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>31</v>
       </c>
@@ -980,18 +1085,18 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E28">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>26</v>
@@ -1000,15 +1105,15 @@
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="E29">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B30">
         <v>26</v>
@@ -1017,81 +1122,337 @@
         <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B32">
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="E32">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E33">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="E34" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>19</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>41</v>
+      </c>
+      <c r="B38">
+        <v>19</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>19</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>43</v>
+      </c>
+      <c r="B40">
+        <v>18</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>44</v>
+      </c>
+      <c r="B41">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>45</v>
+      </c>
+      <c r="B42">
+        <v>17</v>
+      </c>
+      <c r="C42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>46</v>
+      </c>
+      <c r="B43">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>47</v>
+      </c>
+      <c r="B44">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>48</v>
+      </c>
+      <c r="B45">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>49</v>
+      </c>
+      <c r="B46">
+        <v>17</v>
+      </c>
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" t="s">
+        <v>75</v>
+      </c>
+      <c r="E46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>50</v>
+      </c>
+      <c r="B47">
+        <v>16</v>
+      </c>
+      <c r="C47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" t="s">
+        <v>78</v>
+      </c>
+      <c r="E47" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>51</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>52</v>
+      </c>
+      <c r="B49">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made changes to data
</commit_message>
<xml_diff>
--- a/final_WWashington_data_images/Washington_sign_images.xlsx
+++ b/final_WWashington_data_images/Washington_sign_images.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshamakumar/Downloads/5305-DS/Homework/DataScienceProject/final_WWashington_data_images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omkar\Desktop\Data_Science_new_folder\DataScienceProject\final_WWashington_data_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6657C34-967D-5B48-AE58-D613EDEB4D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6998531-BB4A-4BB1-A695-5AC3CA785AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2544" yWindow="2544" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
   <si>
     <t>Number</t>
   </si>
@@ -45,18 +45,12 @@
     <t xml:space="preserve">Image_link   </t>
   </si>
   <si>
-    <t>00001.png</t>
-  </si>
-  <si>
     <t>0002.png</t>
   </si>
   <si>
     <t>0003.png</t>
   </si>
   <si>
-    <t>0004.png</t>
-  </si>
-  <si>
     <t>0005.png</t>
   </si>
   <si>
@@ -274,6 +268,9 @@
   </si>
   <si>
     <t>pedestrian</t>
+  </si>
+  <si>
+    <t>0001.png</t>
   </si>
 </sst>
 </file>
@@ -605,20 +602,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="33.1640625" customWidth="1"/>
+    <col min="2" max="3" width="33.109375" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -646,13 +643,13 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="E2">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -663,13 +660,13 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -680,13 +677,13 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -697,13 +694,13 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -714,15 +711,15 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -731,15 +728,15 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -748,191 +745,191 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
-      </c>
-      <c r="E8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
       <c r="E9">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
       <c r="E10">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
       <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
       <c r="E13">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
         <v>25</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>19</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
       </c>
       <c r="D16" t="s">
         <v>26</v>
       </c>
       <c r="E16">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
       <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
         <v>27</v>
       </c>
-      <c r="D17" t="s">
-        <v>28</v>
-      </c>
       <c r="E17">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
         <v>30</v>
@@ -941,372 +938,372 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>6</v>
       </c>
       <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
         <v>31</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
         <v>32</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>24</v>
-      </c>
-      <c r="B21">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E22">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
         <v>35</v>
       </c>
-      <c r="E23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>27</v>
-      </c>
-      <c r="B24">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24">
         <v>36</v>
       </c>
-      <c r="E24">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>8</v>
       </c>
       <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
         <v>42</v>
       </c>
-      <c r="D26" t="s">
-        <v>38</v>
-      </c>
-      <c r="E26">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>30</v>
-      </c>
-      <c r="B27">
-        <v>8</v>
-      </c>
-      <c r="C27" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>31</v>
-      </c>
-      <c r="B28">
-        <v>9</v>
-      </c>
-      <c r="C28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" t="s">
-        <v>40</v>
-      </c>
       <c r="E28">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
         <v>18</v>
       </c>
-      <c r="D29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>33</v>
-      </c>
-      <c r="B30">
-        <v>26</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>45</v>
       </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>34</v>
-      </c>
-      <c r="B31">
-        <v>25</v>
-      </c>
-      <c r="C31" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" t="s">
-        <v>46</v>
-      </c>
       <c r="E31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E32">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>19</v>
+      </c>
+      <c r="C34" t="s">
         <v>48</v>
-      </c>
-      <c r="E33">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>37</v>
-      </c>
-      <c r="B34">
-        <v>23</v>
-      </c>
-      <c r="C34" t="s">
-        <v>20</v>
       </c>
       <c r="D34" t="s">
         <v>49</v>
       </c>
       <c r="E34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>19</v>
       </c>
       <c r="C35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" t="s">
         <v>50</v>
       </c>
-      <c r="D35" t="s">
-        <v>51</v>
-      </c>
       <c r="E35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>19</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <v>19</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>18</v>
+      </c>
+      <c r="C39" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>42</v>
-      </c>
-      <c r="B39">
-        <v>19</v>
-      </c>
-      <c r="C39" t="s">
-        <v>50</v>
-      </c>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B40">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E40" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B41">
         <v>17</v>
       </c>
       <c r="C41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D41" t="s">
         <v>65</v>
@@ -1315,15 +1312,15 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B42">
         <v>17</v>
       </c>
       <c r="C42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D42" t="s">
         <v>67</v>
@@ -1332,15 +1329,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B43">
         <v>17</v>
       </c>
       <c r="C43" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D43" t="s">
         <v>69</v>
@@ -1349,15 +1346,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B44">
         <v>17</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D44" t="s">
         <v>71</v>
@@ -1366,89 +1363,72 @@
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B45">
         <v>17</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D45" t="s">
         <v>73</v>
       </c>
       <c r="E45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>16</v>
+      </c>
+      <c r="C46" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>49</v>
-      </c>
-      <c r="B46">
-        <v>17</v>
-      </c>
-      <c r="C46" t="s">
-        <v>64</v>
-      </c>
       <c r="D46" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B47">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E47" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B48">
         <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E48" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>52</v>
-      </c>
-      <c r="B49">
-        <v>10</v>
-      </c>
-      <c r="C49" t="s">
-        <v>77</v>
-      </c>
-      <c r="D49" t="s">
-        <v>80</v>
-      </c>
-      <c r="E49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified images as per requirement and deleted some images
</commit_message>
<xml_diff>
--- a/final_WWashington_data_images/Washington_sign_images.xlsx
+++ b/final_WWashington_data_images/Washington_sign_images.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omkar\Desktop\Data_Science_new_folder\DataScienceProject\final_WWashington_data_images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshamakumar/Downloads/5305-DS/Homework/DataScienceProject/final_WWashington_data_images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6998531-BB4A-4BB1-A695-5AC3CA785AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBE9D67-B6FE-3A47-9225-2BBC7FBA1A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2544" yWindow="2544" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="400" yWindow="800" windowWidth="22880" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>Number</t>
   </si>
@@ -84,9 +84,6 @@
     <t>A-2828857</t>
   </si>
   <si>
-    <t>34 maybe</t>
-  </si>
-  <si>
     <t>A-2827768</t>
   </si>
   <si>
@@ -189,88 +186,28 @@
     <t>0042.png</t>
   </si>
   <si>
-    <t>Spped limit 30</t>
-  </si>
-  <si>
-    <t>No pedestrian crossing</t>
-  </si>
-  <si>
-    <t>right turn</t>
-  </si>
-  <si>
-    <t>No parking</t>
-  </si>
-  <si>
-    <t>speed limit 30</t>
-  </si>
-  <si>
     <t>A-2829794</t>
   </si>
   <si>
     <t>0043.png</t>
   </si>
   <si>
-    <t>speed limit 40</t>
-  </si>
-  <si>
     <t>A-2829776</t>
   </si>
   <si>
-    <t>00.44.png</t>
-  </si>
-  <si>
-    <t>right lane end</t>
-  </si>
-  <si>
     <t>0045.png</t>
   </si>
   <si>
-    <t>exit + speed limit 25</t>
-  </si>
-  <si>
-    <t>0046.png</t>
-  </si>
-  <si>
-    <t>exit</t>
-  </si>
-  <si>
-    <t>0047.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stop </t>
-  </si>
-  <si>
-    <t>0048.png</t>
-  </si>
-  <si>
-    <t>speed limit 25</t>
-  </si>
-  <si>
-    <t>0049.png</t>
-  </si>
-  <si>
     <t>A-2829686</t>
   </si>
   <si>
     <t>A-2829398</t>
   </si>
   <si>
-    <t>0050.png</t>
-  </si>
-  <si>
-    <t>0051.png</t>
-  </si>
-  <si>
-    <t>0052.png</t>
-  </si>
-  <si>
-    <t>roundabout</t>
-  </si>
-  <si>
-    <t>pedestrian</t>
-  </si>
-  <si>
     <t>0001.png</t>
+  </si>
+  <si>
+    <t>0044.png</t>
   </si>
 </sst>
 </file>
@@ -602,20 +539,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="33.109375" customWidth="1"/>
+    <col min="2" max="3" width="33.1640625" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="30.77734375" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -632,7 +569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -643,13 +580,13 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E2">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -666,7 +603,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -683,7 +620,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -700,7 +637,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -717,7 +654,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -734,7 +671,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -751,7 +688,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -768,7 +705,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -785,7 +722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -802,7 +739,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -810,16 +747,16 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
         <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
       </c>
       <c r="E12">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -827,16 +764,16 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -844,16 +781,16 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -861,16 +798,16 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -878,16 +815,16 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
         <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>26</v>
       </c>
       <c r="E16">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -895,16 +832,16 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -912,16 +849,16 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -929,16 +866,16 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
         <v>29</v>
-      </c>
-      <c r="D19" t="s">
-        <v>30</v>
       </c>
       <c r="E19">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -946,16 +883,16 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -963,16 +900,16 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -980,16 +917,16 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -997,16 +934,16 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1014,16 +951,16 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1031,16 +968,16 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E25">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1048,16 +985,16 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E26">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1065,16 +1002,16 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E27">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1085,13 +1022,13 @@
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1102,13 +1039,13 @@
         <v>16</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1119,13 +1056,13 @@
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1136,13 +1073,13 @@
         <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E31">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1153,30 +1090,30 @@
         <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E32">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1184,16 +1121,16 @@
         <v>19</v>
       </c>
       <c r="C34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" t="s">
         <v>48</v>
       </c>
-      <c r="D34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1201,234 +1138,115 @@
         <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E35" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
-      </c>
-      <c r="E36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="E36">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D37" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="E37">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C38" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
-      </c>
-      <c r="E38" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="E38">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D39" t="s">
-        <v>60</v>
-      </c>
-      <c r="E39" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="E39">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D40" t="s">
-        <v>63</v>
-      </c>
-      <c r="E40" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="E40">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D41" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42">
-        <v>17</v>
-      </c>
-      <c r="C42" t="s">
-        <v>62</v>
-      </c>
-      <c r="D42" t="s">
-        <v>67</v>
-      </c>
-      <c r="E42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43">
-        <v>17</v>
-      </c>
-      <c r="C43" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" t="s">
-        <v>69</v>
-      </c>
-      <c r="E43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <v>17</v>
-      </c>
-      <c r="C44" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" t="s">
-        <v>71</v>
-      </c>
-      <c r="E44" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>17</v>
-      </c>
-      <c r="C45" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" t="s">
-        <v>73</v>
-      </c>
-      <c r="E45" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46">
-        <v>16</v>
-      </c>
-      <c r="C46" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46" t="s">
-        <v>76</v>
-      </c>
-      <c r="E46" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47">
-        <v>10</v>
-      </c>
-      <c r="C47" t="s">
-        <v>74</v>
-      </c>
-      <c r="D47" t="s">
-        <v>77</v>
-      </c>
-      <c r="E47" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>75</v>
-      </c>
-      <c r="D48" t="s">
-        <v>78</v>
-      </c>
-      <c r="E48" t="s">
-        <v>70</v>
+        <v>56</v>
+      </c>
+      <c r="E41">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added and deleted some images
</commit_message>
<xml_diff>
--- a/final_WWashington_data_images/Washington_sign_images.xlsx
+++ b/final_WWashington_data_images/Washington_sign_images.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshamakumar/Downloads/5305-DS/Homework/DataScienceProject/final_WWashington_data_images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omkar\Desktop\Data_Science_new_folder\DataScienceProject\final_WWashington_data_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBE9D67-B6FE-3A47-9225-2BBC7FBA1A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6518B1B-7BA5-420E-9A8B-A52113CFAD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="800" windowWidth="22880" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
   <si>
     <t>Number</t>
   </si>
@@ -78,9 +78,6 @@
     <t>A-2829033</t>
   </si>
   <si>
-    <t>A-2829014</t>
-  </si>
-  <si>
     <t>A-2828857</t>
   </si>
   <si>
@@ -153,12 +150,6 @@
     <t>0032.png</t>
   </si>
   <si>
-    <t>0033.png</t>
-  </si>
-  <si>
-    <t>0034.png</t>
-  </si>
-  <si>
     <t>0035.png</t>
   </si>
   <si>
@@ -208,6 +199,24 @@
   </si>
   <si>
     <t>0044.png</t>
+  </si>
+  <si>
+    <t>A-2828757</t>
+  </si>
+  <si>
+    <t>0053.png</t>
+  </si>
+  <si>
+    <t>0054.png</t>
+  </si>
+  <si>
+    <t>0055.png</t>
+  </si>
+  <si>
+    <t>0056.png</t>
+  </si>
+  <si>
+    <t>0057.png</t>
   </si>
 </sst>
 </file>
@@ -539,20 +548,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="33.1640625" customWidth="1"/>
+    <col min="2" max="3" width="33.109375" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -569,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -580,13 +589,13 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E2">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -603,7 +612,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -620,7 +629,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -637,7 +646,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -654,7 +663,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -671,7 +680,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -688,7 +697,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -705,7 +714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -722,7 +731,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -739,7 +748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -747,16 +756,16 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
       </c>
       <c r="E12">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -764,16 +773,16 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -781,16 +790,16 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -798,16 +807,16 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -815,16 +824,16 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
         <v>24</v>
-      </c>
-      <c r="D16" t="s">
-        <v>25</v>
       </c>
       <c r="E16">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -832,16 +841,16 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -849,16 +858,16 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -866,16 +875,16 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
         <v>28</v>
-      </c>
-      <c r="D19" t="s">
-        <v>29</v>
       </c>
       <c r="E19">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -883,16 +892,16 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -900,16 +909,16 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -917,16 +926,16 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -934,16 +943,16 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -951,16 +960,16 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -968,16 +977,16 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -985,16 +994,16 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1002,16 +1011,16 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E27">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1022,81 +1031,81 @@
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>26</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E31">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D32" t="s">
         <v>45</v>
       </c>
       <c r="E32">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1104,7 +1113,7 @@
         <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D33" t="s">
         <v>46</v>
@@ -1113,58 +1122,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" t="s">
         <v>47</v>
       </c>
-      <c r="D34" t="s">
-        <v>48</v>
-      </c>
       <c r="E34">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E36">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1172,81 +1181,132 @@
         <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D37" t="s">
         <v>51</v>
       </c>
       <c r="E37">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E38">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C39" t="s">
         <v>55</v>
       </c>
       <c r="D39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E39">
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E40">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
         <v>58</v>
       </c>
       <c r="D41" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E41">
-        <v>14</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>20</v>
+      </c>
+      <c r="C42" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>20</v>
+      </c>
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>